<commit_message>
added skeleton of 2450 guidance
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-cibmtr-additional-peri-transplant-medication.xlsx
+++ b/docs/StructureDefinition-cibmtr-additional-peri-transplant-medication.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="347">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-09-08T13:29:45-05:00</t>
+    <t>2022-11-09T13:32:08-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -253,10 +253,6 @@
   </si>
   <si>
     <t>The US Core Medication Profile is based upon the core FHIR Medication Resource and created to meet the 2015 Edition Common Clinical Data Set 'Medications' requirements.</t>
-  </si>
-  <si>
-    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>NewRx/MedicationPrescribed@@ -280,111 +276,111 @@
     <t>Y</t>
   </si>
   <si>
+    <t xml:space="preserve">id
+</t>
+  </si>
+  <si>
+    <t>Logical id of this artifact</t>
+  </si>
+  <si>
+    <t>The logical id of the resource, as used in the URL for the resource. Once assigned, this value never changes.</t>
+  </si>
+  <si>
+    <t>The only time that a resource does not have an id is when it is being submitted to the server using a create operation.</t>
+  </si>
+  <si>
+    <t>Resource.id</t>
+  </si>
+  <si>
+    <t>Medication.meta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meta
+</t>
+  </si>
+  <si>
+    <t>Metadata about the resource</t>
+  </si>
+  <si>
+    <t>The metadata about the resource. This is content that is maintained by the infrastructure. Changes to the content might not always be associated with version changes to the resource.</t>
+  </si>
+  <si>
+    <t>Resource.meta</t>
+  </si>
+  <si>
+    <t>Medication.meta.id</t>
+  </si>
+  <si>
     <t xml:space="preserve">string
 </t>
   </si>
   <si>
-    <t>Logical id of this artifact</t>
-  </si>
-  <si>
-    <t>The logical id of the resource, as used in the URL for the resource. Once assigned, this value never changes.</t>
-  </si>
-  <si>
-    <t>The only time that a resource does not have an id is when it is being submitted to the server using a create operation.</t>
-  </si>
-  <si>
-    <t>Resource.id</t>
-  </si>
-  <si>
-    <t>Medication.meta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meta
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Medication.meta.extension</t>
+  </si>
+  <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
-    <t>Metadata about the resource</t>
-  </si>
-  <si>
-    <t>The metadata about the resource. This is content that is maintained by the infrastructure. Changes to the content might not always be associated with version changes to the resource.</t>
-  </si>
-  <si>
-    <t>Resource.meta</t>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>Medication.meta.versionId</t>
+  </si>
+  <si>
+    <t>Version specific identifier</t>
+  </si>
+  <si>
+    <t>The version specific identifier, as it appears in the version portion of the URL. This value changes when the resource is created, updated, or deleted.</t>
+  </si>
+  <si>
+    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
+  </si>
+  <si>
+    <t>Meta.versionId</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
-  </si>
-  <si>
-    <t>Medication.meta.id</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>Medication.meta.extension</t>
-  </si>
-  <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>Medication.meta.versionId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id
-</t>
-  </si>
-  <si>
-    <t>Version specific identifier</t>
-  </si>
-  <si>
-    <t>The version specific identifier, as it appears in the version portion of the URL. This value changes when the resource is created, updated, or deleted.</t>
-  </si>
-  <si>
-    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
-  </si>
-  <si>
-    <t>Meta.versionId</t>
   </si>
   <si>
     <t>Medication.meta.lastUpdated</t>
@@ -1686,13 +1682,13 @@
         <v>74</v>
       </c>
       <c r="AI2" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ2" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="AJ2" t="s" s="2">
+      <c r="AK2" t="s" s="2">
         <v>80</v>
-      </c>
-      <c r="AK2" t="s" s="2">
-        <v>81</v>
       </c>
       <c r="AL2" t="s" s="2">
         <v>74</v>
@@ -1703,7 +1699,7 @@
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -1714,28 +1710,28 @@
         <v>75</v>
       </c>
       <c r="F3" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I3" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G3" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I3" t="s" s="2">
+      <c r="J3" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="J3" t="s" s="2">
+      <c r="K3" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="K3" t="s" s="2">
+      <c r="L3" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="L3" t="s" s="2">
+      <c r="M3" t="s" s="2">
         <v>87</v>
-      </c>
-      <c r="M3" t="s" s="2">
-        <v>88</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" t="s" s="2">
@@ -1785,13 +1781,13 @@
         <v>74</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AF3" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>74</v>
@@ -1814,7 +1810,7 @@
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
@@ -1825,25 +1821,25 @@
         <v>75</v>
       </c>
       <c r="F4" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I4" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G4" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H4" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I4" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J4" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="K4" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="K4" t="s" s="2">
+      <c r="L4" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="L4" t="s" s="2">
-        <v>93</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1894,19 +1890,19 @@
         <v>74</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH4" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>74</v>
@@ -1923,7 +1919,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -1934,7 +1930,7 @@
         <v>75</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>74</v>
@@ -1946,13 +1942,13 @@
         <v>74</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="K5" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="L5" t="s" s="2">
         <v>97</v>
-      </c>
-      <c r="L5" t="s" s="2">
-        <v>98</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -2003,25 +1999,25 @@
         <v>74</v>
       </c>
       <c r="AE5" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AF5" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG5" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH5" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI5" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ5" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK5" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="AF5" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG5" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH5" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI5" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ5" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK5" t="s" s="2">
-        <v>100</v>
       </c>
       <c r="AL5" t="s" s="2">
         <v>74</v>
@@ -2032,11 +2028,11 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
@@ -2055,16 +2051,16 @@
         <v>74</v>
       </c>
       <c r="J6" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="K6" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="K6" t="s" s="2">
+      <c r="L6" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="L6" t="s" s="2">
+      <c r="M6" t="s" s="2">
         <v>105</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>106</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -2102,19 +2098,19 @@
         <v>74</v>
       </c>
       <c r="AA6" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="AB6" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="AB6" t="s" s="2">
+      <c r="AC6" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD6" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="AC6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD6" t="s" s="2">
+      <c r="AE6" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>110</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>75</v>
@@ -2126,13 +2122,13 @@
         <v>74</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AL6" t="s" s="2">
         <v>74</v>
@@ -2143,7 +2139,7 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
@@ -2154,28 +2150,28 @@
         <v>75</v>
       </c>
       <c r="F7" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G7" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H7" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G7" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H7" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I7" t="s" s="2">
+      <c r="J7" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="J7" t="s" s="2">
+      <c r="K7" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="L7" t="s" s="2">
         <v>113</v>
       </c>
-      <c r="K7" t="s" s="2">
+      <c r="M7" t="s" s="2">
         <v>114</v>
-      </c>
-      <c r="L7" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="M7" t="s" s="2">
-        <v>116</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -2225,19 +2221,19 @@
         <v>74</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG7" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH7" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ7" t="s" s="2">
         <v>74</v>
@@ -2254,7 +2250,7 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -2265,28 +2261,28 @@
         <v>75</v>
       </c>
       <c r="F8" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G8" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H8" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I8" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G8" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H8" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I8" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J8" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="K8" t="s" s="2">
         <v>119</v>
       </c>
-      <c r="K8" t="s" s="2">
+      <c r="L8" t="s" s="2">
         <v>120</v>
       </c>
-      <c r="L8" t="s" s="2">
+      <c r="M8" t="s" s="2">
         <v>121</v>
-      </c>
-      <c r="M8" t="s" s="2">
-        <v>122</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2336,19 +2332,19 @@
         <v>74</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH8" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ8" t="s" s="2">
         <v>74</v>
@@ -2365,7 +2361,7 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -2376,28 +2372,28 @@
         <v>75</v>
       </c>
       <c r="F9" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G9" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H9" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I9" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G9" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H9" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I9" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J9" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="K9" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="K9" t="s" s="2">
+      <c r="L9" t="s" s="2">
         <v>126</v>
       </c>
-      <c r="L9" t="s" s="2">
+      <c r="M9" t="s" s="2">
         <v>127</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>128</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2447,19 +2443,19 @@
         <v>74</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG9" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH9" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>74</v>
@@ -2476,7 +2472,7 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -2496,19 +2492,19 @@
         <v>74</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J10" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="K10" t="s" s="2">
         <v>131</v>
       </c>
-      <c r="K10" t="s" s="2">
+      <c r="L10" t="s" s="2">
         <v>132</v>
       </c>
-      <c r="L10" t="s" s="2">
+      <c r="M10" t="s" s="2">
         <v>133</v>
-      </c>
-      <c r="M10" t="s" s="2">
-        <v>134</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
@@ -2558,7 +2554,7 @@
         <v>74</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>75</v>
@@ -2570,7 +2566,7 @@
         <v>74</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>74</v>
@@ -2587,7 +2583,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -2595,7 +2591,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>76</v>
@@ -2607,19 +2603,19 @@
         <v>74</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J11" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="K11" t="s" s="2">
         <v>137</v>
       </c>
-      <c r="K11" t="s" s="2">
+      <c r="L11" t="s" s="2">
         <v>138</v>
       </c>
-      <c r="L11" t="s" s="2">
+      <c r="M11" t="s" s="2">
         <v>139</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>140</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
@@ -2645,31 +2641,31 @@
         <v>74</v>
       </c>
       <c r="W11" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="X11" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="X11" t="s" s="2">
+      <c r="Y11" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="Y11" t="s" s="2">
+      <c r="Z11" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA11" t="s" s="2">
         <v>143</v>
       </c>
-      <c r="Z11" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA11" t="s" s="2">
+      <c r="AB11" t="s" s="2">
         <v>144</v>
       </c>
-      <c r="AB11" t="s" s="2">
+      <c r="AC11" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD11" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="AE11" t="s" s="2">
         <v>145</v>
-      </c>
-      <c r="AC11" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD11" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="AE11" t="s" s="2">
-        <v>146</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>75</v>
@@ -2681,7 +2677,7 @@
         <v>74</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>74</v>
@@ -2698,41 +2694,41 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C12" t="s" s="2">
         <v>74</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="F12" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G12" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="F12" t="s" s="2">
+      <c r="H12" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I12" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G12" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="H12" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I12" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J12" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="K12" t="s" s="2">
         <v>137</v>
       </c>
-      <c r="K12" t="s" s="2">
+      <c r="L12" t="s" s="2">
         <v>138</v>
       </c>
-      <c r="L12" t="s" s="2">
+      <c r="M12" t="s" s="2">
         <v>139</v>
-      </c>
-      <c r="M12" t="s" s="2">
-        <v>140</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -2758,14 +2754,14 @@
         <v>74</v>
       </c>
       <c r="W12" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="X12" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="X12" t="s" s="2">
+      <c r="Y12" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="Y12" t="s" s="2">
-        <v>143</v>
-      </c>
       <c r="Z12" t="s" s="2">
         <v>74</v>
       </c>
@@ -2782,7 +2778,7 @@
         <v>74</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>75</v>
@@ -2794,7 +2790,7 @@
         <v>74</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ12" t="s" s="2">
         <v>74</v>
@@ -2811,7 +2807,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2822,7 +2818,7 @@
         <v>75</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>74</v>
@@ -2834,13 +2830,13 @@
         <v>74</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="K13" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="L13" t="s" s="2">
         <v>97</v>
-      </c>
-      <c r="L13" t="s" s="2">
-        <v>98</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2891,25 +2887,25 @@
         <v>74</v>
       </c>
       <c r="AE13" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AF13" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG13" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK13" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="AF13" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG13" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK13" t="s" s="2">
-        <v>100</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>74</v>
@@ -2920,11 +2916,11 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
@@ -2943,16 +2939,16 @@
         <v>74</v>
       </c>
       <c r="J14" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="K14" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="K14" t="s" s="2">
+      <c r="L14" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="L14" t="s" s="2">
+      <c r="M14" t="s" s="2">
         <v>105</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>106</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -2990,19 +2986,19 @@
         <v>74</v>
       </c>
       <c r="AA14" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="AB14" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="AB14" t="s" s="2">
+      <c r="AC14" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD14" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="AC14" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD14" t="s" s="2">
+      <c r="AE14" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AE14" t="s" s="2">
-        <v>110</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>75</v>
@@ -3014,13 +3010,13 @@
         <v>74</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ14" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>74</v>
@@ -3031,7 +3027,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3039,34 +3035,34 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="F15" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I15" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="F15" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="G15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I15" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J15" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K15" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="L15" t="s" s="2">
         <v>151</v>
       </c>
-      <c r="L15" t="s" s="2">
+      <c r="M15" t="s" s="2">
         <v>152</v>
       </c>
-      <c r="M15" t="s" s="2">
+      <c r="N15" t="s" s="2">
         <v>153</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>154</v>
       </c>
       <c r="O15" t="s" s="2">
         <v>74</v>
@@ -3076,75 +3072,75 @@
         <v>74</v>
       </c>
       <c r="R15" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="S15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE15" t="s" s="2">
         <v>155</v>
       </c>
-      <c r="S15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="T15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="U15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="V15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="W15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Z15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE15" t="s" s="2">
+      <c r="AF15" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG15" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI15" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="AJ15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK15" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="AF15" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG15" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI15" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AJ15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK15" t="s" s="2">
+      <c r="AL15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM15" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="AL15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM15" t="s" s="2">
-        <v>158</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -3155,28 +3151,28 @@
         <v>75</v>
       </c>
       <c r="F16" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H16" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I16" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G16" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H16" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I16" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J16" t="s" s="2">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="L16" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="L16" t="s" s="2">
+      <c r="M16" t="s" s="2">
         <v>161</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>162</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -3226,36 +3222,36 @@
         <v>74</v>
       </c>
       <c r="AE16" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AF16" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG16" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH16" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI16" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="AJ16" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK16" t="s" s="2">
         <v>163</v>
       </c>
-      <c r="AF16" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG16" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH16" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI16" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AJ16" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK16" t="s" s="2">
+      <c r="AL16" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM16" t="s" s="2">
         <v>164</v>
-      </c>
-      <c r="AL16" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM16" t="s" s="2">
-        <v>165</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3263,32 +3259,32 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="F17" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G17" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H17" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I17" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="F17" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="G17" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H17" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I17" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J17" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>167</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>168</v>
-      </c>
-      <c r="L17" t="s" s="2">
-        <v>169</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" t="s" s="2">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>74</v>
@@ -3337,36 +3333,36 @@
         <v>74</v>
       </c>
       <c r="AE17" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="AF17" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG17" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH17" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI17" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>171</v>
       </c>
-      <c r="AF17" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG17" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH17" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI17" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AJ17" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK17" t="s" s="2">
+      <c r="AL17" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM17" t="s" s="2">
         <v>172</v>
-      </c>
-      <c r="AL17" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM17" t="s" s="2">
-        <v>173</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3377,29 +3373,29 @@
         <v>75</v>
       </c>
       <c r="F18" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H18" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I18" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G18" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H18" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I18" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J18" t="s" s="2">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="K18" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="L18" t="s" s="2">
         <v>175</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>176</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" t="s" s="2">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>74</v>
@@ -3448,36 +3444,36 @@
         <v>74</v>
       </c>
       <c r="AE18" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="AF18" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG18" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH18" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI18" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="AJ18" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK18" t="s" s="2">
         <v>178</v>
       </c>
-      <c r="AF18" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG18" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH18" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI18" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AJ18" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK18" t="s" s="2">
+      <c r="AL18" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM18" t="s" s="2">
         <v>179</v>
-      </c>
-      <c r="AL18" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM18" t="s" s="2">
-        <v>180</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3488,31 +3484,31 @@
         <v>75</v>
       </c>
       <c r="F19" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G19" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H19" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I19" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G19" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H19" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I19" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J19" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>182</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="L19" t="s" s="2">
         <v>183</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>184</v>
       </c>
-      <c r="M19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>185</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>186</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>74</v>
@@ -3561,36 +3557,36 @@
         <v>74</v>
       </c>
       <c r="AE19" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="AF19" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG19" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH19" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI19" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="AJ19" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK19" t="s" s="2">
         <v>187</v>
       </c>
-      <c r="AF19" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG19" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH19" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI19" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AJ19" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK19" t="s" s="2">
+      <c r="AL19" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM19" t="s" s="2">
         <v>188</v>
-      </c>
-      <c r="AL19" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM19" t="s" s="2">
-        <v>189</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3610,19 +3606,19 @@
         <v>74</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K20" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="L20" t="s" s="2">
         <v>191</v>
       </c>
-      <c r="L20" t="s" s="2">
+      <c r="M20" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3648,31 +3644,31 @@
         <v>74</v>
       </c>
       <c r="W20" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="X20" t="s" s="2">
         <v>194</v>
       </c>
-      <c r="X20" t="s" s="2">
+      <c r="Y20" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="Y20" t="s" s="2">
+      <c r="Z20" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA20" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB20" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC20" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD20" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE20" t="s" s="2">
         <v>196</v>
-      </c>
-      <c r="Z20" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA20" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB20" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC20" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD20" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE20" t="s" s="2">
-        <v>197</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>75</v>
@@ -3684,7 +3680,7 @@
         <v>74</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ20" t="s" s="2">
         <v>74</v>
@@ -3701,7 +3697,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3712,28 +3708,28 @@
         <v>75</v>
       </c>
       <c r="F21" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G21" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H21" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G21" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H21" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="I21" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3783,19 +3779,19 @@
         <v>74</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH21" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>74</v>
@@ -3812,7 +3808,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3823,7 +3819,7 @@
         <v>75</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>74</v>
@@ -3835,16 +3831,16 @@
         <v>74</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="L22" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="L22" t="s" s="2">
+      <c r="M22" t="s" s="2">
         <v>205</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>206</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
@@ -3870,43 +3866,43 @@
         <v>74</v>
       </c>
       <c r="W22" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="X22" t="s" s="2">
         <v>207</v>
       </c>
-      <c r="X22" t="s" s="2">
+      <c r="Y22" t="s" s="2">
         <v>208</v>
       </c>
-      <c r="Y22" t="s" s="2">
+      <c r="Z22" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA22" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB22" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC22" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD22" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE22" t="s" s="2">
         <v>209</v>
       </c>
-      <c r="Z22" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA22" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB22" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC22" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD22" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE22" t="s" s="2">
-        <v>210</v>
-      </c>
       <c r="AF22" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>74</v>
@@ -3923,18 +3919,18 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>75</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>74</v>
@@ -3946,16 +3942,16 @@
         <v>74</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="K23" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="L23" t="s" s="2">
         <v>214</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>215</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>216</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -4005,25 +4001,25 @@
         <v>74</v>
       </c>
       <c r="AE23" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="AF23" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG23" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH23" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI23" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="AJ23" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK23" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="AF23" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG23" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH23" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI23" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AJ23" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK23" t="s" s="2">
-        <v>218</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>74</v>
@@ -4034,11 +4030,11 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4057,16 +4053,16 @@
         <v>74</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="K24" t="s" s="2">
         <v>221</v>
       </c>
-      <c r="K24" t="s" s="2">
+      <c r="L24" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="M24" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -4116,7 +4112,7 @@
         <v>74</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>75</v>
@@ -4134,7 +4130,7 @@
         <v>74</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>74</v>
@@ -4145,11 +4141,11 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -4168,16 +4164,16 @@
         <v>74</v>
       </c>
       <c r="J25" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="K25" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="K25" t="s" s="2">
-        <v>104</v>
-      </c>
       <c r="L25" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -4227,7 +4223,7 @@
         <v>74</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>75</v>
@@ -4239,13 +4235,13 @@
         <v>74</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>74</v>
@@ -4256,11 +4252,11 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -4273,25 +4269,25 @@
         <v>74</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I26" t="s" s="2">
         <v>74</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="N26" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>74</v>
@@ -4340,7 +4336,7 @@
         <v>74</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>75</v>
@@ -4352,13 +4348,13 @@
         <v>74</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ26" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>74</v>
@@ -4369,7 +4365,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4389,19 +4385,19 @@
         <v>74</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J27" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="K27" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="K27" t="s" s="2">
+      <c r="L27" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="L27" t="s" s="2">
+      <c r="M27" t="s" s="2">
         <v>238</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>239</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4451,7 +4447,7 @@
         <v>74</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>75</v>
@@ -4463,16 +4459,16 @@
         <v>74</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AL27" t="s" s="2">
         <v>240</v>
-      </c>
-      <c r="AL27" t="s" s="2">
-        <v>241</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>74</v>
@@ -4480,7 +4476,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4488,31 +4484,31 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="F28" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G28" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="F28" t="s" s="2">
+      <c r="H28" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I28" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G28" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="H28" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I28" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J28" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="K28" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="K28" t="s" s="2">
+      <c r="L28" t="s" s="2">
         <v>244</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>245</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>246</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4538,58 +4534,58 @@
         <v>74</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X28" s="2"/>
       <c r="Y28" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="Z28" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA28" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB28" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC28" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD28" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE28" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="AF28" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG28" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH28" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI28" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="AJ28" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="Z28" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA28" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB28" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC28" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD28" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE28" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="AF28" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG28" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH28" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI28" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AJ28" t="s" s="2">
+      <c r="AK28" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="AK28" t="s" s="2">
+      <c r="AL28" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="AL28" t="s" s="2">
+      <c r="AM28" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="AM28" t="s" s="2">
-        <v>251</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4600,7 +4596,7 @@
         <v>75</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>74</v>
@@ -4612,13 +4608,13 @@
         <v>74</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>97</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>98</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4669,25 +4665,25 @@
         <v>74</v>
       </c>
       <c r="AE29" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK29" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="AF29" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI29" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK29" t="s" s="2">
-        <v>100</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>74</v>
@@ -4698,11 +4694,11 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
@@ -4721,16 +4717,16 @@
         <v>74</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>105</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>106</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4768,19 +4764,19 @@
         <v>74</v>
       </c>
       <c r="AA30" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="AB30" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="AB30" t="s" s="2">
+      <c r="AC30" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD30" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="AC30" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD30" t="s" s="2">
+      <c r="AE30" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AE30" t="s" s="2">
-        <v>110</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>75</v>
@@ -4792,13 +4788,13 @@
         <v>74</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>74</v>
@@ -4809,7 +4805,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4829,22 +4825,22 @@
         <v>74</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>255</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="M31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>257</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>258</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>74</v>
@@ -4869,29 +4865,29 @@
         <v>74</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X31" s="2"/>
       <c r="Y31" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="Z31" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA31" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB31" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC31" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD31" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE31" t="s" s="2">
         <v>259</v>
-      </c>
-      <c r="Z31" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA31" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB31" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC31" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD31" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE31" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>75</v>
@@ -4903,24 +4899,24 @@
         <v>74</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK31" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="AL31" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM31" t="s" s="2">
         <v>261</v>
-      </c>
-      <c r="AL31" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>262</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4931,31 +4927,31 @@
         <v>75</v>
       </c>
       <c r="F32" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G32" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H32" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I32" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G32" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H32" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I32" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J32" t="s" s="2">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="L32" t="s" s="2">
+      <c r="M32" t="s" s="2">
         <v>265</v>
       </c>
-      <c r="M32" t="s" s="2">
+      <c r="N32" t="s" s="2">
         <v>266</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>267</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>74</v>
@@ -5004,36 +5000,36 @@
         <v>74</v>
       </c>
       <c r="AE32" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="AF32" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG32" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH32" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI32" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK32" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="AF32" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG32" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH32" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI32" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AJ32" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK32" t="s" s="2">
+      <c r="AL32" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM32" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="AL32" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM32" t="s" s="2">
-        <v>270</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5044,28 +5040,28 @@
         <v>75</v>
       </c>
       <c r="F33" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G33" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H33" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G33" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H33" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="I33" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>272</v>
       </c>
-      <c r="L33" t="s" s="2">
+      <c r="M33" t="s" s="2">
         <v>273</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>274</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
@@ -5091,49 +5087,49 @@
         <v>74</v>
       </c>
       <c r="W33" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="X33" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="X33" t="s" s="2">
+      <c r="Y33" t="s" s="2">
         <v>276</v>
       </c>
-      <c r="Y33" t="s" s="2">
+      <c r="Z33" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA33" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB33" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC33" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD33" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE33" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="AF33" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG33" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH33" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI33" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="AJ33" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK33" t="s" s="2">
         <v>277</v>
-      </c>
-      <c r="Z33" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA33" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB33" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC33" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD33" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE33" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="AF33" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG33" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH33" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI33" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AJ33" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK33" t="s" s="2">
-        <v>278</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>74</v>
@@ -5144,7 +5140,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5155,25 +5151,25 @@
         <v>75</v>
       </c>
       <c r="F34" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G34" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H34" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I34" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G34" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H34" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I34" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J34" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="K34" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="K34" t="s" s="2">
+      <c r="L34" t="s" s="2">
         <v>281</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>282</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5224,36 +5220,36 @@
         <v>74</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ34" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="AK34" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="AK34" t="s" s="2">
+      <c r="AL34" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="AL34" t="s" s="2">
+      <c r="AM34" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="AM34" t="s" s="2">
-        <v>286</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5264,7 +5260,7 @@
         <v>75</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>74</v>
@@ -5276,16 +5272,16 @@
         <v>74</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>288</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>289</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>290</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
@@ -5311,60 +5307,60 @@
         <v>74</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="X35" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="Y35" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="Y35" t="s" s="2">
+      <c r="Z35" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA35" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB35" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC35" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD35" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE35" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="AF35" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG35" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH35" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI35" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
         <v>292</v>
       </c>
-      <c r="Z35" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA35" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB35" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC35" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD35" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE35" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="AF35" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG35" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH35" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI35" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AJ35" t="s" s="2">
+      <c r="AK35" t="s" s="2">
         <v>293</v>
       </c>
-      <c r="AK35" t="s" s="2">
+      <c r="AL35" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>294</v>
-      </c>
-      <c r="AL35" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>295</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5375,25 +5371,25 @@
         <v>75</v>
       </c>
       <c r="F36" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="G36" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H36" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I36" t="s" s="2">
         <v>83</v>
       </c>
-      <c r="G36" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H36" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I36" t="s" s="2">
-        <v>84</v>
-      </c>
       <c r="J36" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="K36" t="s" s="2">
         <v>297</v>
       </c>
-      <c r="K36" t="s" s="2">
+      <c r="L36" t="s" s="2">
         <v>298</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>299</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5444,25 +5440,25 @@
         <v>74</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH36" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>74</v>
@@ -5473,7 +5469,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5496,16 +5492,16 @@
         <v>74</v>
       </c>
       <c r="J37" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="K37" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="K37" t="s" s="2">
+      <c r="L37" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>304</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -5555,7 +5551,7 @@
         <v>74</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>75</v>
@@ -5567,13 +5563,13 @@
         <v>74</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>74</v>
@@ -5584,7 +5580,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5595,7 +5591,7 @@
         <v>75</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>74</v>
@@ -5607,13 +5603,13 @@
         <v>74</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>97</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>98</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5664,25 +5660,25 @@
         <v>74</v>
       </c>
       <c r="AE38" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AF38" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG38" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH38" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI38" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ38" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK38" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="AF38" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG38" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH38" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI38" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ38" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>100</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>74</v>
@@ -5693,11 +5689,11 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -5716,16 +5712,16 @@
         <v>74</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="L39" t="s" s="2">
+      <c r="M39" t="s" s="2">
         <v>105</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>106</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
@@ -5775,7 +5771,7 @@
         <v>74</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>75</v>
@@ -5787,13 +5783,13 @@
         <v>74</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>74</v>
@@ -5804,11 +5800,11 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -5821,25 +5817,25 @@
         <v>74</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="L40" t="s" s="2">
-        <v>312</v>
-      </c>
       <c r="M40" t="s" s="2">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>74</v>
@@ -5888,7 +5884,7 @@
         <v>74</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>75</v>
@@ -5900,13 +5896,13 @@
         <v>74</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>74</v>
@@ -5917,7 +5913,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5925,10 +5921,10 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>74</v>
@@ -5940,17 +5936,17 @@
         <v>74</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="K41" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="K41" t="s" s="2">
+      <c r="L41" t="s" s="2">
         <v>316</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>317</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>74</v>
@@ -5999,36 +5995,36 @@
         <v>74</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AK41" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="AL41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM41" t="s" s="2">
         <v>319</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>320</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6039,7 +6035,7 @@
         <v>75</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>74</v>
@@ -6051,17 +6047,17 @@
         <v>74</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>74</v>
@@ -6110,25 +6106,25 @@
         <v>74</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>74</v>
@@ -6139,7 +6135,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6150,7 +6146,7 @@
         <v>75</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>74</v>
@@ -6162,13 +6158,13 @@
         <v>74</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6219,36 +6215,36 @@
         <v>74</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ43" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="AK43" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="AL43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM43" t="s" s="2">
         <v>329</v>
-      </c>
-      <c r="AK43" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="AL43" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM43" t="s" s="2">
-        <v>330</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6259,7 +6255,7 @@
         <v>75</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>74</v>
@@ -6271,13 +6267,13 @@
         <v>74</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6328,25 +6324,25 @@
         <v>74</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>74</v>
@@ -6357,7 +6353,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6368,7 +6364,7 @@
         <v>75</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>74</v>
@@ -6380,13 +6376,13 @@
         <v>74</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>97</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>98</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6437,25 +6433,25 @@
         <v>74</v>
       </c>
       <c r="AE45" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AF45" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG45" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK45" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="AF45" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AG45" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AH45" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI45" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ45" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK45" t="s" s="2">
-        <v>100</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>74</v>
@@ -6466,11 +6462,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6489,16 +6485,16 @@
         <v>74</v>
       </c>
       <c r="J46" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="K46" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="K46" t="s" s="2">
+      <c r="L46" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="L46" t="s" s="2">
+      <c r="M46" t="s" s="2">
         <v>105</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>106</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6548,7 +6544,7 @@
         <v>74</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>75</v>
@@ -6560,13 +6556,13 @@
         <v>74</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>74</v>
@@ -6577,11 +6573,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6594,25 +6590,25 @@
         <v>74</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="L47" t="s" s="2">
-        <v>312</v>
-      </c>
       <c r="M47" t="s" s="2">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>74</v>
@@ -6661,7 +6657,7 @@
         <v>74</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>75</v>
@@ -6673,13 +6669,13 @@
         <v>74</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>74</v>
@@ -6690,7 +6686,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6701,7 +6697,7 @@
         <v>75</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>74</v>
@@ -6713,13 +6709,13 @@
         <v>74</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>339</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>340</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6770,36 +6766,36 @@
         <v>74</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6810,7 +6806,7 @@
         <v>75</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>74</v>
@@ -6822,13 +6818,13 @@
         <v>74</v>
       </c>
       <c r="J49" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="K49" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="K49" t="s" s="2">
+      <c r="L49" t="s" s="2">
         <v>344</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>345</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6879,31 +6875,31 @@
         <v>74</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AK49" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="AL49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AM49" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="AL49" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AM49" t="s" s="2">
-        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cytogenetics profile and example
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-cibmtr-additional-peri-transplant-medication.xlsx
+++ b/docs/StructureDefinition-cibmtr-additional-peri-transplant-medication.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-11-09T14:05:34-06:00</t>
+    <t>2022-11-10T14:39:35-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -500,7 +500,7 @@
     <t>Need to be unambiguous about the source of the definition of the symbol.</t>
   </si>
   <si>
-    <t>http://terminology.nmdp.org/codesystem/transplant-center</t>
+    <t>http://terminology.cibmtr.org/codesystem/transplant-center</t>
   </si>
   <si>
     <t>Coding.system</t>

</xml_diff>

<commit_message>
updated footer background color
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-cibmtr-additional-peri-transplant-medication.xlsx
+++ b/docs/StructureDefinition-cibmtr-additional-peri-transplant-medication.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-05-04T09:48:28-05:00</t>
+    <t>2023-05-04T21:27:58-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1463,17 +1463,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="52.19921875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="37.84765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="16.578125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.8984375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="51.0703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="37.21875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="16.44140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="31.81640625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="30.390625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1482,25 +1482,25 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.7109375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="95.77734375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="75.94140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.984375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.30078125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="9.04296875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="95.2265625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="77.71875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="40.0859375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="195.390625" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="95.72265625" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="32.84375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="194.96484375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="95.25" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="33.05078125" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="255.0" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>

</xml_diff>